<commit_message>
updated .html pages to include viz
</commit_message>
<xml_diff>
--- a/data/fulldata.xlsx
+++ b/data/fulldata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\OneDrive\Desktop\digit494\bobdylan494\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960E2B2-12C2-42A3-9BF1-5013B985D65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F10209-AD59-4B92-95F1-FBFBC006CE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="78" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1327,7 +1327,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23BFE698-EC48-46AD-9113-AE11C8053FD3}" name="PivotTable20" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23BFE698-EC48-46AD-9113-AE11C8053FD3}" name="PivotTable20" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
   <location ref="A3" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -1847,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1371A4-FC25-45A0-BA5E-16ABB1D212BD}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,16 +3757,6 @@
       </c>
       <c r="R34">
         <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R35">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R36">
-        <v>10.878787880000001</v>
       </c>
     </row>
   </sheetData>
@@ -3844,7 +3834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3E6A2-BA2C-427E-A327-1A2D0F7FBBD7}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:U3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CSV export of full album data 1st tab only for Kumu
</commit_message>
<xml_diff>
--- a/data/fulldata.xlsx
+++ b/data/fulldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\OneDrive\Desktop\digit494\bobdylan494\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eeb4/Documents/GitHub/newtfire/494Projects/bobdylan494/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7960E2B2-12C2-42A3-9BF1-5013B985D65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A15BD15-1CA1-FE45-B937-CED116A86BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
+    <workbookView xWindow="-34720" yWindow="-7980" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="78" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1327,7 +1327,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23BFE698-EC48-46AD-9113-AE11C8053FD3}" name="PivotTable20" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23BFE698-EC48-46AD-9113-AE11C8053FD3}" name="PivotTable20" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
   <location ref="A3" firstHeaderRow="0" firstDataRow="0" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -1816,13 +1816,13 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1830,12 +1830,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1847,15 +1847,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1371A4-FC25-45A0-BA5E-16ABB1D212BD}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -3757,16 +3757,6 @@
       </c>
       <c r="R34">
         <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R35">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R36">
-        <v>10.878787880000001</v>
       </c>
     </row>
   </sheetData>
@@ -3782,9 +3772,9 @@
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3801,7 +3791,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>17</v>
       </c>
@@ -3818,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>16</v>
       </c>
@@ -3844,13 +3834,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3E6A2-BA2C-427E-A327-1A2D0F7FBBD7}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3915,7 +3905,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
@@ -3980,7 +3970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
updated svg and html pages
</commit_message>
<xml_diff>
--- a/data/fulldata.xlsx
+++ b/data/fulldata.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\OneDrive\Desktop\digit494\bobdylan494\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001C74D9-861D-42F4-BCF0-2BBE7BAE6CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7622B06-42CF-4DAA-8C2F-AF9BF22427EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{9ECD06F7-3C19-431E-AED8-AF4D03A60475}"/>
   </bookViews>
   <sheets>
-    <sheet name="fulldata" sheetId="1" r:id="rId1"/>
-    <sheet name="AntConc Data" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <sheet name="fulldata" sheetId="1" r:id="rId2"/>
+    <sheet name="AntConc Data" sheetId="7" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="90" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="96">
   <si>
     <t>Album</t>
   </si>
@@ -322,6 +326,12 @@
   </si>
   <si>
     <t>Avg. Verses</t>
+  </si>
+  <si>
+    <t>Count of Format</t>
+  </si>
+  <si>
+    <t>Vinyl</t>
   </si>
 </sst>
 </file>
@@ -357,8 +367,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,6 +405,9 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="1">
+          <cell r="A1" t="str">
+            <v>AlbumName</v>
+          </cell>
           <cell r="E1" t="str">
             <v>ReleaseYear</v>
           </cell>
@@ -1299,6 +1316,866 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Samantha Moniot" refreshedDate="45773.743615856481" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="33" xr:uid="{EEF7DEE3-B430-488C-8F1D-4D98EC680DA4}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:S34" sheet="fulldata"/>
+  </cacheSource>
+  <cacheFields count="19">
+    <cacheField name="Album" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Release Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1962" maxValue="2020"/>
+    </cacheField>
+    <cacheField name="Period" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Early Dylan"/>
+        <s v="Late Dylan"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="AlbumType" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Format" numFmtId="0">
+      <sharedItems count="1">
+        <s v="vinyl"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Format 2" numFmtId="0">
+      <sharedItems count="5">
+        <s v="None"/>
+        <s v="eight-track"/>
+        <s v="cassette"/>
+        <s v="CD"/>
+        <s v="digital"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Format 3" numFmtId="0">
+      <sharedItems count="3">
+        <s v="None"/>
+        <s v="cassette"/>
+        <s v="CD"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Length" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="27.14" maxValue="73.150000000000006"/>
+    </cacheField>
+    <cacheField name="Genre" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Genre2" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Genre3" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Genre4" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Genre5" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Instrument 1" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Instrument 2" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Instrument 3" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Instrument 4" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Instrument 5" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Track Count" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="24"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="33">
+  <r>
+    <s v="Bob Dylan"/>
+    <n v="1962"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="36.54"/>
+    <s v="folk"/>
+    <s v="country blues"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <s v="The Freewheelin’ Bob Dylan"/>
+    <n v="1963"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="50.04"/>
+    <s v="folk"/>
+    <s v="blues"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <s v="The Times They Are A-Changin’"/>
+    <n v="1964"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="45.36"/>
+    <s v="folk"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Another Side of Bob Dylan"/>
+    <n v="1964"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="50.37"/>
+    <s v="folk"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Bringing it All Back Home"/>
+    <n v="1965"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="47.21"/>
+    <s v="folk"/>
+    <s v="folk rock"/>
+    <s v="blues"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Keyboards"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Highway 61 Revisited"/>
+    <n v="1965"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="51.26"/>
+    <s v=" folk rock"/>
+    <s v="blues rock"/>
+    <s v="rock and roll"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="Slide Whistle"/>
+    <s v="None"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="Blonde on Blonde"/>
+    <n v="1966"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="72.569999999999993"/>
+    <s v=" folk rock"/>
+    <s v="blues rock"/>
+    <s v="country rock"/>
+    <s v="rock and roll"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <s v="John Wesley Harding"/>
+    <n v="1967"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="38.24"/>
+    <s v=" folk rock"/>
+    <s v="country rock"/>
+    <s v="roots rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <s v="Nashville Skyline"/>
+    <n v="1969"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="27.14"/>
+    <s v="country rock"/>
+    <s v="country"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Keyboards"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Self Portrait"/>
+    <n v="1970"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="73.150000000000006"/>
+    <s v="folk rock"/>
+    <s v="blues rock"/>
+    <s v="country rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Keyboards"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <s v="New Morning"/>
+    <n v="1970"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="35.21"/>
+    <s v=" folk rock"/>
+    <s v="country rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Acoustic Guitar"/>
+    <s v="Electric Guitar"/>
+    <s v="Piano"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <s v="Pat Garrett &amp; Billy the Kid"/>
+    <n v="1973"/>
+    <x v="0"/>
+    <s v="comp"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="35.229999999999997"/>
+    <s v=" folk rock"/>
+    <s v="country rock"/>
+    <s v="soundtrack"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Planet Waves"/>
+    <n v="1974"/>
+    <x v="0"/>
+    <s v="live"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="42.12"/>
+    <s v="roots rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Blood on the Tracks"/>
+    <n v="1975"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="51.42"/>
+    <s v="folk"/>
+    <s v="folk rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Organ"/>
+    <s v="Mandolin"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Desire"/>
+    <n v="1976"/>
+    <x v="0"/>
+    <s v="live"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="56.13"/>
+    <s v="folk rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="Street-Legal"/>
+    <n v="1978"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="50.18"/>
+    <s v="rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="Slow Train Coming"/>
+    <n v="1979"/>
+    <x v="0"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="46.19"/>
+    <s v="Christian rock"/>
+    <s v="blues rock"/>
+    <s v="gospel"/>
+    <s v="funk"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="Saved"/>
+    <n v="1980"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="42.39"/>
+    <s v="Christian rock"/>
+    <s v="gospel"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="Shot of Love"/>
+    <n v="1981"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="44.27"/>
+    <s v="Christian rock"/>
+    <s v="gospel"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Infidels"/>
+    <n v="1983"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="41.39"/>
+    <s v="folk rock"/>
+    <s v="heartland rock"/>
+    <s v="reggae"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="Empire Burlesque"/>
+    <n v="1985"/>
+    <x v="1"/>
+    <s v="comp"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="46.24"/>
+    <s v="blues rock"/>
+    <s v="gospel"/>
+    <s v="pop"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Keyboards"/>
+    <s v="Piano"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Knocked Out Loaded"/>
+    <n v="1986"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="35.18"/>
+    <s v="rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Keyboards"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="Down In The Groove"/>
+    <n v="1988"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="32.1"/>
+    <s v="rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Oh Mercy"/>
+    <n v="1989"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="38.46"/>
+    <s v="rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="twelve-string guitar"/>
+    <s v="Hammond Organ"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Under The Red Sky"/>
+    <n v="1990"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="38.46"/>
+    <s v="rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="Accordion"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Good As I Been To You"/>
+    <n v="1992"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="55.31"/>
+    <s v="folk"/>
+    <s v="blues"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <s v="World Gone Wrong"/>
+    <n v="1993"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="43.51"/>
+    <s v="folk"/>
+    <s v="blues"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Time Out of Mind"/>
+    <n v="1997"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="72.5"/>
+    <s v="blues rock"/>
+    <s v="country"/>
+    <s v="blues"/>
+    <s v="rockabilly"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Love and Theft"/>
+    <n v="2001"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="57.25"/>
+    <s v="roots rock"/>
+    <s v="americana"/>
+    <s v="blues"/>
+    <s v="country"/>
+    <s v="jazz"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <s v="Modern Times"/>
+    <n v="2006"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="63.04"/>
+    <s v="folk rock"/>
+    <s v="americana"/>
+    <s v="blues"/>
+    <s v="rockabilly"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Together Through Life"/>
+    <n v="2009"/>
+    <x v="1"/>
+    <s v="comp"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="45.33"/>
+    <s v="folk rock"/>
+    <s v="blues rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Keyboards"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Tempest"/>
+    <n v="2012"/>
+    <x v="1"/>
+    <s v="og"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="68.31"/>
+    <s v="folk"/>
+    <s v="folk rock"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Piano"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="Rough and Rowdy Ways"/>
+    <n v="2020"/>
+    <x v="1"/>
+    <s v="comp"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="70.33"/>
+    <s v="folk"/>
+    <s v="blues rock"/>
+    <s v="americana"/>
+    <s v="rhythm and blues"/>
+    <s v="None"/>
+    <s v="Guitar"/>
+    <s v="Harmonica"/>
+    <s v="None"/>
+    <s v="None"/>
+    <s v="None"/>
+    <n v="10"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6ECB7ED-F5AC-45DA-B4CB-5468CE3D7476}" name="PivotTable1" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:A4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="19">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="2" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Format" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1617,11 +2494,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6667DDD-1095-47B6-8B5A-0322AE05A643}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1371A4-FC25-45A0-BA5E-16ABB1D212BD}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3667,15 +4619,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7176C1-87CC-4529-B835-5CDBBB526EDB}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3860,6 +4813,20 @@
         <v>6.2</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>SUM(A2:A9)</f>
+        <v>498</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ref="B10:C10" si="0">SUM(B2:B9)</f>
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>429.37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>